<commit_message>
PROS-13119 Rename oral to oral care category
</commit_message>
<xml_diff>
--- a/Projects/GSKSG/Data/gsk_set_up.xlsx
+++ b/Projects/GSKSG/Data/gsk_set_up.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Functional KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">Include</t>
   </si>
   <si>
-    <t xml:space="preserve">Oral ,Pain</t>
+    <t xml:space="preserve">Oral Care ,Pain</t>
   </si>
   <si>
     <t xml:space="preserve">Exclude</t>
@@ -93,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -130,12 +130,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -200,7 +194,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,10 +229,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -324,30 +314,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1014" min="12" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.78542510121457"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="12" style="1" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -398,7 +388,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -422,7 +412,7 @@
         <v>15</v>
       </c>
       <c r="K2" s="7"/>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="AMA2" s="0"/>
@@ -482,7 +472,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>